<commit_message>
generate to take from stock file
</commit_message>
<xml_diff>
--- a/master/output/slit_plan_M75_BAO.xlsx
+++ b/master/output/slit_plan_M75_BAO.xlsx
@@ -22,43 +22,43 @@
     <t>Width-2 (mm)</t>
   </si>
   <si>
+    <t>Extra Width Generated (mm)</t>
+  </si>
+  <si>
+    <t>Trim (mm)</t>
+  </si>
+  <si>
+    <t>Mother Coil Width (mm)</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Mother Coil Weight (kg)</t>
+  </si>
+  <si>
+    <t>Mother Coil Length (m)</t>
+  </si>
+  <si>
+    <t>Weight-1 (kg)</t>
+  </si>
+  <si>
+    <t>Weight-2 (kg)</t>
+  </si>
+  <si>
+    <t>Extra Weight (kg)</t>
+  </si>
+  <si>
     <t>Width-3 (mm)</t>
   </si>
   <si>
     <t>Width-4 (mm)</t>
   </si>
   <si>
-    <t>Extra Width Generated (mm)</t>
-  </si>
-  <si>
-    <t>Trim (mm)</t>
-  </si>
-  <si>
-    <t>Mother Coil Width (mm)</t>
-  </si>
-  <si>
-    <t>Grade</t>
-  </si>
-  <si>
-    <t>Mother Coil Weight (kg)</t>
-  </si>
-  <si>
-    <t>Mother Coil Length (m)</t>
-  </si>
-  <si>
-    <t>Weight-1 (kg)</t>
-  </si>
-  <si>
-    <t>Weight-2 (kg)</t>
-  </si>
-  <si>
     <t>Weight-3 (kg)</t>
   </si>
   <si>
     <t>Weight-4 (kg)</t>
-  </si>
-  <si>
-    <t>Extra Weight (kg)</t>
   </si>
   <si>
     <t>M75_BAO</t>
@@ -477,49 +477,49 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>110</v>
+        <v>180</v>
       </c>
       <c r="C2">
-        <v>130</v>
+        <v>190</v>
       </c>
       <c r="D2">
-        <v>180</v>
+        <v>320</v>
       </c>
       <c r="E2">
-        <v>190</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>80</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
+        <v>700</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
       </c>
       <c r="H2">
-        <v>700</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
+        <v>1000</v>
+      </c>
+      <c r="I2">
+        <v>822.6491771451605</v>
       </c>
       <c r="J2">
-        <v>1000</v>
+        <v>257.1428571428571</v>
       </c>
       <c r="K2">
-        <v>822.6491771451605</v>
+        <v>271.4285714285714</v>
       </c>
       <c r="L2">
-        <v>157.1428571428571</v>
+        <v>457.1428571428572</v>
       </c>
       <c r="M2">
-        <v>185.7142857142857</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>257.1428571428571</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>271.4285714285714</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>114.2857142857143</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -527,49 +527,49 @@
         <v>1</v>
       </c>
       <c r="B3">
+        <v>110</v>
+      </c>
+      <c r="C3">
+        <v>130</v>
+      </c>
+      <c r="D3">
+        <v>140</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>710</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>1500</v>
+      </c>
+      <c r="I3">
+        <v>1216.593853524533</v>
+      </c>
+      <c r="J3">
+        <v>232.394366197183</v>
+      </c>
+      <c r="K3">
+        <v>274.6478873239437</v>
+      </c>
+      <c r="L3">
+        <v>295.7746478873239</v>
+      </c>
+      <c r="M3">
         <v>150</v>
       </c>
-      <c r="C3">
+      <c r="N3">
         <v>170</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>380</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>710</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3">
-        <v>1500</v>
-      </c>
-      <c r="K3">
-        <v>1216.593853524533</v>
-      </c>
-      <c r="L3">
+      <c r="O3">
         <v>316.9014084507042</v>
       </c>
-      <c r="M3">
+      <c r="P3">
         <v>359.1549295774648</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>802.8169014084507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>